<commit_message>
Committed with maven integration.
</commit_message>
<xml_diff>
--- a/result/Summary.xlsx
+++ b/result/Summary.xlsx
@@ -527,10 +527,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>